<commit_message>
updated with materials from software engineering training
</commit_message>
<xml_diff>
--- a/data/trainings.xlsx
+++ b/data/trainings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>date</t>
   </si>
@@ -173,6 +173,18 @@
   <si>
     <t>20220913_gsd_adaptive.html</t>
   </si>
+  <si>
+    <t>Good Software Engineering Practice for R Packages</t>
+  </si>
+  <si>
+    <t>Kevin Kunzmann, Friedrich Pahlke, Daniel Sabanés Bové</t>
+  </si>
+  <si>
+    <t>forward.html</t>
+  </si>
+  <si>
+    <t>Boehringer Ingelheim, rpact, Roche</t>
+  </si>
 </sst>
 </file>
 
@@ -309,7 +321,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -337,7 +349,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -631,11 +643,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L952"/>
+  <dimension ref="A1:L953"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,132 +695,131 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="str">
+        <f>"10.02.2023"</f>
+        <v>10.02.2023</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="10"/>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="str">
         <f>"13.09.2022"</f>
         <v>13.09.2022</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="str">
-        <f>"29.03.2022"</f>
-        <v>29.03.2022</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5">
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
+      <c r="H3" s="5" t="s">
+        <v>48</v>
       </c>
-      <c r="I3" t="s">
-        <v>30</v>
+      <c r="I3" s="3" t="s">
+        <v>49</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
         <f>"29.03.2022"</f>
         <v>29.03.2022</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="str">
+        <f>"29.03.2022"</f>
+        <v>29.03.2022</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
         <v>2</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="str">
+      <c r="K5" s="18"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="str">
         <f>"21.02.2022"</f>
         <v>21.02.2022</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="18"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="str">
-        <f t="shared" ref="A6:A8" si="0">"21.02.2022"</f>
-        <v>21.02.2022</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>36</v>
@@ -817,17 +828,17 @@
         <v>9</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A7:A9" si="0">"21.02.2022"</f>
         <v>21.02.2022</v>
       </c>
       <c r="B7" s="4"/>
@@ -835,7 +846,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>36</v>
@@ -844,10 +855,10 @@
         <v>9</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="3"/>
@@ -862,7 +873,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>36</v>
@@ -871,67 +882,69 @@
         <v>9</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K8" s="18"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="str">
-        <f>"02.02.2021"</f>
-        <v>02.02.2021</v>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>21.02.2022</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5">
+        <v>4</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="4">
-        <v>1</v>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>13</v>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>11</v>
+      <c r="I9" s="5" t="s">
+        <v>42</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>14</v>
+      <c r="J9" s="5" t="s">
+        <v>43</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>18</v>
-      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
         <f>"02.02.2021"</f>
         <v>02.02.2021</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>15</v>
+      <c r="G10" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>16</v>
+      <c r="I10" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
         <f>"02.02.2021"</f>
         <v>02.02.2021</v>
@@ -941,49 +954,53 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
-        <f>"19.08.2019"</f>
-        <v>19.08.2019</v>
+        <f>"02.02.2021"</f>
+        <v>02.02.2021</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+      <c r="H12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
-        <f>"01.03.2018"</f>
-        <v>01.03.2018</v>
+        <f>"19.08.2019"</f>
+        <v>19.08.2019</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="6"/>
@@ -992,38 +1009,47 @@
         <v>1</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="57" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
+        <f>"01.03.2018"</f>
+        <v>01.03.2018</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="str">
         <f>"05.06.2014"</f>
         <v>05.06.2014</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="4">
+      <c r="C15" s="4"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="4">
         <v>1</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="4"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1102,11 +1128,11 @@
       <c r="J21" s="16"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="4"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -1117,8 +1143,8 @@
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="4"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -1134,6 +1160,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1145,7 +1172,6 @@
       <c r="F25" s="4"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
       <c r="J25" s="16"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1168,8 +1194,8 @@
       <c r="E27" s="6"/>
       <c r="F27" s="4"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
       <c r="J27" s="16"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1180,7 +1206,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="4"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="H28" s="17"/>
       <c r="I28" s="17"/>
       <c r="J28" s="16"/>
     </row>
@@ -1191,9 +1217,9 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="17"/>
+      <c r="G29" s="6"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1203,8 +1229,8 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="16"/>
     </row>
@@ -1217,7 +1243,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="6"/>
       <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
+      <c r="I31" s="6"/>
       <c r="J31" s="16"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1239,9 +1265,9 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
       <c r="J33" s="16"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1253,7 +1279,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="17"/>
       <c r="H34" s="6"/>
-      <c r="I34" s="4"/>
+      <c r="I34" s="6"/>
       <c r="J34" s="16"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1263,34 +1289,34 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="6"/>
       <c r="I35" s="4"/>
       <c r="J35" s="16"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="16"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="4"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="16"/>
+      <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
@@ -1350,7 +1376,7 @@
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="J42" s="16"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
@@ -1370,7 +1396,7 @@
       <c r="C44" s="8"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
-      <c r="F44" s="2"/>
+      <c r="F44" s="4"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="1"/>
@@ -1402,8 +1428,8 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="2"/>
@@ -1450,8 +1476,8 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="2"/>
@@ -1462,8 +1488,8 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="2"/>
@@ -1558,8 +1584,8 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="F60" s="2"/>
@@ -2925,16 +2951,16 @@
       <c r="J173" s="1"/>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A174" s="14"/>
-      <c r="B174" s="9"/>
-      <c r="C174" s="9"/>
-      <c r="D174" s="5"/>
-      <c r="E174" s="5"/>
-      <c r="F174" s="3"/>
+      <c r="A174" s="13"/>
+      <c r="B174" s="8"/>
+      <c r="C174" s="8"/>
+      <c r="D174" s="6"/>
+      <c r="E174" s="6"/>
+      <c r="F174" s="2"/>
       <c r="G174" s="5"/>
       <c r="H174" s="5"/>
-      <c r="I174" s="3"/>
-      <c r="J174" s="3"/>
+      <c r="I174" s="1"/>
+      <c r="J174" s="1"/>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="14"/>
@@ -12272,6 +12298,18 @@
       <c r="I952" s="3"/>
       <c r="J952" s="3"/>
     </row>
+    <row r="953" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A953" s="14"/>
+      <c r="B953" s="9"/>
+      <c r="C953" s="9"/>
+      <c r="D953" s="5"/>
+      <c r="E953" s="5"/>
+      <c r="F953" s="3"/>
+      <c r="G953" s="5"/>
+      <c r="H953" s="5"/>
+      <c r="I953" s="3"/>
+      <c r="J953" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
removed slide deck 'Do you speak statistics?' again, per Youyou's request (12/8/2023)
</commit_message>
<xml_diff>
--- a/data/trainings.xlsx
+++ b/data/trainings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F9D6F9-7821-44ED-ADD2-2D8B29A8D87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFDA0F7-249E-4010-BA0D-766CB784DA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>date</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>Novartis</t>
-  </si>
-  <si>
-    <t>Do you speak statistics - BBS Next Gen 2023-12-06.pdf</t>
   </si>
   <si>
     <t>Lukas A. Widmer, Michael Mayer</t>
@@ -705,7 +702,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,9 +773,7 @@
       <c r="I2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="str">
@@ -795,16 +790,16 @@
         <v>2</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="K3" s="18"/>
     </row>

</xml_diff>